<commit_message>
Added WAV Trigger software
</commit_message>
<xml_diff>
--- a/Third Party Software/Third Party Software Index.xlsx
+++ b/Third Party Software/Third Party Software Index.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Software</t>
   </si>
@@ -55,6 +55,42 @@
   </si>
   <si>
     <t>Version</t>
+  </si>
+  <si>
+    <t>WAV Trigger Firmware</t>
+  </si>
+  <si>
+    <t>WAV Trigger</t>
+  </si>
+  <si>
+    <t>http://robertsonics.com/wav-trigger-downloads/</t>
+  </si>
+  <si>
+    <t>Firmware for WAV Trigger</t>
+  </si>
+  <si>
+    <t>WAV Trigger Firmware Update Utility</t>
+  </si>
+  <si>
+    <t>Firmware updater for WAV Trigger</t>
+  </si>
+  <si>
+    <t>WAV Trigger Init File Maker Utility</t>
+  </si>
+  <si>
+    <t>Init File Maker for WAV Trigger</t>
+  </si>
+  <si>
+    <t>WAV Trigger Serial Control Utility</t>
+  </si>
+  <si>
+    <t>Serial Control Utility for WAV Trigger</t>
+  </si>
+  <si>
+    <t>WAV Trigger Online Guide</t>
+  </si>
+  <si>
+    <t>http://robertsonics.com/wav-trigger-online-user-guide/</t>
   </si>
 </sst>
 </file>
@@ -388,20 +424,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="21.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -459,6 +495,103 @@
       </c>
       <c r="F3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1">
+        <v>41746</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1">
+        <v>41746</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.02</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1">
+        <v>41746</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.02</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1">
+        <v>41746</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1">
+        <v>41746</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated third party software index
</commit_message>
<xml_diff>
--- a/Third Party Software/Third Party Software Index.xlsx
+++ b/Third Party Software/Third Party Software Index.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>Software</t>
   </si>
@@ -91,13 +91,22 @@
   </si>
   <si>
     <t>http://robertsonics.com/wav-trigger-online-user-guide/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sabertooth/Syren </t>
+  </si>
+  <si>
+    <t>http://www.dimensionengineering.com/info/arduino</t>
+  </si>
+  <si>
+    <t>Drivers for Syren 10 and Sabertooth 2x25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +145,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -214,6 +228,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -248,6 +263,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -423,24 +439,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="21.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -477,7 +493,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -497,7 +513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -517,7 +533,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -537,7 +553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -557,7 +573,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -577,7 +593,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -592,6 +608,23 @@
       </c>
       <c r="F8" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>41748</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -601,24 +634,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>